<commit_message>
all done with CAR and SDG watersheds
</commit_message>
<xml_diff>
--- a/2 - Flow output Excel files - working drafts/Data Output 08_31_2019/Offsets and Clip times 08_31_2019.xlsx
+++ b/2 - Flow output Excel files - working drafts/Data Output 08_31_2019/Offsets and Clip times 08_31_2019.xlsx
@@ -10794,8 +10794,8 @@
   </sheetPr>
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="24.9" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>